<commit_message>
Newest update on 21st July
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\70073624\09_Supervising\Tien_Pham\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlotte/Documents/Programming - Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B2F1F2-0909-4748-B1A4-DE06F3547668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="756" windowWidth="30240" windowHeight="17136" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment 1" sheetId="1" r:id="rId1"/>
     <sheet name="Experiment 2" sheetId="2" r:id="rId2"/>
     <sheet name="Experiment 3" sheetId="3" r:id="rId3"/>
     <sheet name="Experiment 5" sheetId="4" r:id="rId4"/>
+    <sheet name="Experiment 0" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="35">
   <si>
     <t>Experiment #1 100 mL/min - 20 mg/mL glucose</t>
   </si>
@@ -132,11 +134,23 @@
   <si>
     <t>average flow rate</t>
   </si>
+  <si>
+    <t>start solution, after 4h</t>
+  </si>
+  <si>
+    <t>t=240</t>
+  </si>
+  <si>
+    <t>&lt;0,21</t>
+  </si>
+  <si>
+    <t>Experiment #0: 20 mg/mL glucose; 0 mM phosphate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -294,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -419,13 +433,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -517,17 +559,22 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -843,16 +890,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -879,7 +926,7 @@
       <c r="V1" s="15"/>
       <c r="W1" s="15"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -936,7 +983,7 @@
       </c>
       <c r="Y2" s="31"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -992,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1048,7 +1095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1112,7 +1159,7 @@
       </c>
       <c r="W5" s="5"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -1180,7 +1227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1248,7 +1295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
@@ -1300,7 +1347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
@@ -1368,7 +1415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
@@ -1436,7 +1483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1444,41 +1491,41 @@
         <v>75.125</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="68" t="s">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="69">
-        <v>1</v>
-      </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="69">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="70">
+        <v>1</v>
+      </c>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="70">
         <v>2</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1492,16 +1539,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
@@ -1528,7 +1575,7 @@
       <c r="V1" s="17"/>
       <c r="W1" s="17"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1584,7 +1631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1640,7 +1687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1696,7 +1743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
@@ -1760,7 +1807,7 @@
       </c>
       <c r="W5" s="18"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>14</v>
       </c>
@@ -1828,7 +1875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>16</v>
       </c>
@@ -1896,7 +1943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>17</v>
       </c>
@@ -1942,7 +1989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>18</v>
       </c>
@@ -2010,7 +2057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>19</v>
       </c>
@@ -2078,18 +2125,43 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="71">
-        <v>72</v>
-      </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K20" s="28"/>
+      <c r="B13" s="68">
+        <v>123</v>
+      </c>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+    </row>
+    <row r="19" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+    </row>
+    <row r="20" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2098,16 +2170,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>25</v>
       </c>
@@ -2136,7 +2208,7 @@
       <c r="X1" s="35"/>
       <c r="Y1" s="35"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -2198,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +2332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -2322,7 +2394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>13</v>
       </c>
@@ -2392,7 +2464,7 @@
       </c>
       <c r="Y5" s="38"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
         <v>14</v>
       </c>
@@ -2466,7 +2538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>16</v>
       </c>
@@ -2509,7 +2581,7 @@
       <c r="O7" s="43">
         <v>0.59</v>
       </c>
-      <c r="P7" s="70">
+      <c r="P7" s="67">
         <v>0.2</v>
       </c>
       <c r="Q7" s="42">
@@ -2540,7 +2612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
         <v>17</v>
       </c>
@@ -2592,7 +2664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
         <v>18</v>
       </c>
@@ -2666,7 +2738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
         <v>19</v>
       </c>
@@ -2740,18 +2812,47 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="71">
-        <v>72</v>
-      </c>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L20" s="67"/>
+      <c r="B13" s="68">
+        <v>78.182000000000002</v>
+      </c>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K14" s="71"/>
+      <c r="L14" s="71"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+    </row>
+    <row r="17" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+    </row>
+    <row r="18" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
+    </row>
+    <row r="19" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+    </row>
+    <row r="20" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+    </row>
+    <row r="21" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2760,16 +2861,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>28</v>
       </c>
@@ -2797,7 +2898,7 @@
       <c r="W1" s="49"/>
       <c r="X1" s="49"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -2856,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -2915,7 +3016,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -2974,7 +3075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>13</v>
       </c>
@@ -3041,7 +3142,7 @@
       </c>
       <c r="X5" s="55"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="56" t="s">
         <v>14</v>
       </c>
@@ -3112,7 +3213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
         <v>16</v>
       </c>
@@ -3183,7 +3284,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="62" t="s">
         <v>17</v>
       </c>
@@ -3254,7 +3355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="s">
         <v>18</v>
       </c>
@@ -3325,7 +3426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
         <v>19</v>
       </c>
@@ -3396,12 +3497,635 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="68">
         <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4333D61F-7C91-1F4F-8891-CC154DAF55E9}">
+  <dimension ref="A1:X13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="71"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" t="s">
+        <v>11</v>
+      </c>
+      <c r="U4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.3756944444444445</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.37638888888888888</v>
+      </c>
+      <c r="D5" s="73">
+        <v>0.37777777777777799</v>
+      </c>
+      <c r="E5" s="73">
+        <v>0.37916666666666599</v>
+      </c>
+      <c r="F5" s="73">
+        <v>0.38055555555555498</v>
+      </c>
+      <c r="G5" s="73">
+        <v>0.38194444444444398</v>
+      </c>
+      <c r="H5" s="73">
+        <v>0.38333333333333303</v>
+      </c>
+      <c r="I5" s="74">
+        <v>0.38472222222222202</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.38611111111111002</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="M5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.3756944444444445</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.37708333333333299</v>
+      </c>
+      <c r="P5" s="73">
+        <v>0.37847222222222199</v>
+      </c>
+      <c r="Q5" s="73">
+        <v>0.37986111111111098</v>
+      </c>
+      <c r="R5" s="73">
+        <v>0.38124999999999998</v>
+      </c>
+      <c r="S5" s="73">
+        <v>0.38263888888888797</v>
+      </c>
+      <c r="T5" s="73">
+        <v>0.38402777777777702</v>
+      </c>
+      <c r="U5" s="74">
+        <v>0.38541666666666602</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.38611111111111002</v>
+      </c>
+      <c r="W5" s="5"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7">
+        <v>30.9</v>
+      </c>
+      <c r="C6" s="6">
+        <v>31</v>
+      </c>
+      <c r="D6" s="6">
+        <v>31.4</v>
+      </c>
+      <c r="E6" s="6">
+        <v>30.9</v>
+      </c>
+      <c r="F6" s="6">
+        <v>31</v>
+      </c>
+      <c r="G6" s="6">
+        <v>30.8</v>
+      </c>
+      <c r="H6" s="6">
+        <v>31</v>
+      </c>
+      <c r="I6" s="6">
+        <v>30.4</v>
+      </c>
+      <c r="J6" s="7">
+        <v>30.3</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="7">
+        <v>30.9</v>
+      </c>
+      <c r="O6" s="6">
+        <v>31</v>
+      </c>
+      <c r="P6" s="6">
+        <v>31.2</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>30.1</v>
+      </c>
+      <c r="R6" s="6">
+        <v>30.7</v>
+      </c>
+      <c r="S6" s="6">
+        <v>30.8</v>
+      </c>
+      <c r="T6" s="6">
+        <v>30.6</v>
+      </c>
+      <c r="U6" s="6">
+        <v>30.5</v>
+      </c>
+      <c r="V6" s="7">
+        <v>30.3</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.59</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="S7" s="8">
+        <v>0.43</v>
+      </c>
+      <c r="T7" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="U7" s="8">
+        <v>0.48</v>
+      </c>
+      <c r="V7" s="9">
+        <v>0.59</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="12">
+        <v>137</v>
+      </c>
+      <c r="C8" s="11">
+        <v>139</v>
+      </c>
+      <c r="D8" s="11">
+        <v>139</v>
+      </c>
+      <c r="E8" s="11">
+        <v>138</v>
+      </c>
+      <c r="F8" s="11">
+        <v>138</v>
+      </c>
+      <c r="G8" s="11">
+        <v>138</v>
+      </c>
+      <c r="H8" s="11">
+        <v>138</v>
+      </c>
+      <c r="I8" s="11">
+        <v>138</v>
+      </c>
+      <c r="J8" s="12">
+        <v>139</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="12">
+        <v>137</v>
+      </c>
+      <c r="O8" s="11">
+        <v>141</v>
+      </c>
+      <c r="P8" s="11">
+        <v>140</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>140</v>
+      </c>
+      <c r="R8" s="11">
+        <v>140</v>
+      </c>
+      <c r="S8" s="11">
+        <v>139</v>
+      </c>
+      <c r="T8" s="11">
+        <v>139</v>
+      </c>
+      <c r="U8" s="11">
+        <v>139</v>
+      </c>
+      <c r="V8" s="12">
+        <v>139</v>
+      </c>
+      <c r="W8" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1.34</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.86</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1.04</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1.22</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1.32</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1.35</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1.4</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="9">
+        <v>1.34</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="P9" s="8">
+        <v>0.66</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="R9" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="S9" s="8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="T9" s="8">
+        <v>1.21</v>
+      </c>
+      <c r="U9" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="V9" s="9">
+        <v>1.4</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="76">
+        <v>106.9</v>
+      </c>
+      <c r="C10" s="75">
+        <v>5.7</v>
+      </c>
+      <c r="D10" s="75">
+        <v>37.4</v>
+      </c>
+      <c r="E10" s="75">
+        <v>68.3</v>
+      </c>
+      <c r="F10" s="75">
+        <v>98.7</v>
+      </c>
+      <c r="G10" s="75">
+        <v>106.1</v>
+      </c>
+      <c r="H10" s="75">
+        <v>107.2</v>
+      </c>
+      <c r="I10" s="75">
+        <v>106.2</v>
+      </c>
+      <c r="J10" s="76">
+        <v>106.5</v>
+      </c>
+      <c r="K10" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="76">
+        <v>106.9</v>
+      </c>
+      <c r="O10" s="75">
+        <v>1.9</v>
+      </c>
+      <c r="P10" s="75">
+        <v>11.7</v>
+      </c>
+      <c r="Q10" s="75">
+        <v>27.1</v>
+      </c>
+      <c r="R10" s="75">
+        <v>55</v>
+      </c>
+      <c r="S10" s="75">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="T10" s="75">
+        <v>86</v>
+      </c>
+      <c r="U10" s="75">
+        <v>89.5</v>
+      </c>
+      <c r="V10" s="76">
+        <v>106.5</v>
+      </c>
+      <c r="W10" s="75" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="32">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>